<commit_message>
enable auto filer in the testing file
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/filters-conditionalFormatting.xlsx
+++ b/src/main/webapp/book/filters-conditionalFormatting.xlsx
@@ -63,14 +63,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -78,13 +78,13 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -184,21 +184,21 @@
     <xf numFmtId="14" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 4" xfId="1" builtinId="19"/>
@@ -500,27 +500,27 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.19921875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.796875" customWidth="1"/>
+    <col min="6" max="6" width="18.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="2"/>
@@ -549,270 +549,271 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>42384</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>13</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>89500</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>62600</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <f>C4-D4</f>
         <v>26900</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="12">
         <f>E4</f>
         <v>26900</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>42415</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>19</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>100500</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>60300</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <f t="shared" ref="E5:E15" si="0">C5-D5</f>
         <v>40200</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <f>E4+E5</f>
         <v>67100</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>42444</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>25</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>119200</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>27800</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <f t="shared" si="0"/>
         <v>91400</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <f>E4+E5+E6</f>
         <v>158500</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>42475</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>22</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>115900</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>79600</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <f>C7-D7</f>
         <v>36300</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <f>E7</f>
         <v>36300</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>42505</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>28</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>123700</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>84000</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <f t="shared" si="0"/>
         <v>39700</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <f>E7+E8</f>
         <v>76000</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>42536</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>35</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>129300</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>83100</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <f t="shared" si="0"/>
         <v>46200</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <f>E7+E8+E9</f>
         <v>122200</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>42566</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>20</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>110700</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>77300</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <f t="shared" si="0"/>
         <v>33400</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <f>E10</f>
         <v>33400</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>42597</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>31</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>125100</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>85500</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <f t="shared" si="0"/>
         <v>39600</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <f>E10+E11</f>
         <v>73000</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>42628</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>27</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>120100</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>78900</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <f t="shared" si="0"/>
         <v>41200</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="14">
         <f>E10+E11+E12</f>
         <v>114200</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>42658</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>24</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>118400</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <v>91000</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <f t="shared" si="0"/>
         <v>27400</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="15">
         <f>E13</f>
         <v>27400</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>42689</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>19</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>100300</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="10">
         <v>65100</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <f t="shared" si="0"/>
         <v>35200</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="15">
         <f>E13+E14</f>
         <v>62600</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
+      <c r="A15" s="8">
         <v>42719</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>17</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>94200</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="10">
         <v>65800</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="11">
         <f t="shared" si="0"/>
         <v>28400</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="15">
         <f>E13+E14+E15</f>
         <v>91000</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:F15"/>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>

</xml_diff>